<commit_message>
Information on Batteries and Launches for Programs added to Notes
</commit_message>
<xml_diff>
--- a/Notes/Battery/Battery Information.xlsx
+++ b/Notes/Battery/Battery Information.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pap\Dropbox\GAMES\KSP\Git\RP-0\Notes\Battery\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pap\Dropbox\GAMES\KSP\Git\RP-1\Notes\Battery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{98185A69-E7C5-4141-B490-82BA66A7CB59}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E5D554-035D-4FC1-AF83-AD9B4BAE43B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11925" xr2:uid="{6C14037C-793E-4394-BC97-FD3DB9E55288}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6C14037C-793E-4394-BC97-FD3DB9E55288}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="KSP Power" sheetId="3" r:id="rId2"/>
     <sheet name="References" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -584,7 +595,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>

</xml_diff>